<commit_message>
Bug fix to elec/DRC
</commit_message>
<xml_diff>
--- a/InputData/elec/DRC/Demand Response Capacity.xlsx
+++ b/InputData/elec/DRC/Demand Response Capacity.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-us\InputData\elec\DRC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -72,9 +72,6 @@
     <t>Time (Year)</t>
   </si>
   <si>
-    <t>Peak Power Demand : MostRecentRun</t>
-  </si>
-  <si>
     <t>Peak Demand - EPS Output</t>
   </si>
   <si>
@@ -88,6 +85,9 @@
   </si>
   <si>
     <t>We then scale the potential from 2030 to 2050 by the growth in peak demand (EPS model output).</t>
+  </si>
+  <si>
+    <t>Peak Power Demand after Storage and DR[summer] : MostRecentRun</t>
   </si>
 </sst>
 </file>
@@ -546,12 +546,12 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
@@ -559,12 +559,12 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" s="6"/>
     </row>
@@ -625,12 +625,12 @@
   <dimension ref="A1:AH7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="AH6" sqref="AH6:AH7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="1" max="1" width="17.9296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.45">
@@ -658,7 +658,7 @@
     </row>
     <row r="5" spans="1:34" s="11" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.45">
@@ -666,208 +666,203 @@
         <v>15</v>
       </c>
       <c r="B6">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C6">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="D6">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="E6">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="F6">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="G6">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="H6">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="I6">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="J6">
-        <v>2026</v>
+        <v>2027</v>
       </c>
       <c r="K6">
-        <v>2027</v>
+        <v>2028</v>
       </c>
       <c r="L6">
-        <v>2028</v>
+        <v>2029</v>
       </c>
       <c r="M6">
-        <v>2029</v>
+        <v>2030</v>
       </c>
       <c r="N6">
-        <v>2030</v>
+        <v>2031</v>
       </c>
       <c r="O6">
-        <v>2031</v>
+        <v>2032</v>
       </c>
       <c r="P6">
-        <v>2032</v>
+        <v>2033</v>
       </c>
       <c r="Q6">
-        <v>2033</v>
+        <v>2034</v>
       </c>
       <c r="R6">
-        <v>2034</v>
+        <v>2035</v>
       </c>
       <c r="S6">
-        <v>2035</v>
+        <v>2036</v>
       </c>
       <c r="T6">
-        <v>2036</v>
+        <v>2037</v>
       </c>
       <c r="U6">
-        <v>2037</v>
+        <v>2038</v>
       </c>
       <c r="V6">
-        <v>2038</v>
+        <v>2039</v>
       </c>
       <c r="W6">
-        <v>2039</v>
+        <v>2040</v>
       </c>
       <c r="X6">
-        <v>2040</v>
+        <v>2041</v>
       </c>
       <c r="Y6">
-        <v>2041</v>
+        <v>2042</v>
       </c>
       <c r="Z6">
-        <v>2042</v>
+        <v>2043</v>
       </c>
       <c r="AA6">
-        <v>2043</v>
+        <v>2044</v>
       </c>
       <c r="AB6">
-        <v>2044</v>
+        <v>2045</v>
       </c>
       <c r="AC6">
-        <v>2045</v>
+        <v>2046</v>
       </c>
       <c r="AD6">
-        <v>2046</v>
+        <v>2047</v>
       </c>
       <c r="AE6">
-        <v>2047</v>
+        <v>2048</v>
       </c>
       <c r="AF6">
-        <v>2048</v>
+        <v>2049</v>
       </c>
       <c r="AG6">
-        <v>2049</v>
-      </c>
-      <c r="AH6">
         <v>2050</v>
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B7">
-        <v>855335</v>
+        <v>752136</v>
       </c>
       <c r="C7">
-        <v>860978</v>
+        <v>683006</v>
       </c>
       <c r="D7">
-        <v>829114</v>
+        <v>728954</v>
       </c>
       <c r="E7">
-        <v>858530</v>
+        <v>745991</v>
       </c>
       <c r="F7">
-        <v>873258</v>
+        <v>757422</v>
       </c>
       <c r="G7">
-        <v>882009</v>
+        <v>766081</v>
       </c>
       <c r="H7">
-        <v>888855</v>
+        <v>772495</v>
       </c>
       <c r="I7">
-        <v>895021</v>
+        <v>776739</v>
       </c>
       <c r="J7">
-        <v>900356</v>
+        <v>779659</v>
       </c>
       <c r="K7">
-        <v>906369</v>
+        <v>784465</v>
       </c>
       <c r="L7">
-        <v>914175</v>
+        <v>792336</v>
       </c>
       <c r="M7">
-        <v>922266</v>
+        <v>796481</v>
       </c>
       <c r="N7">
-        <v>928730</v>
+        <v>800947</v>
       </c>
       <c r="O7">
-        <v>936606</v>
+        <v>806133</v>
       </c>
       <c r="P7">
-        <v>944847</v>
+        <v>810368</v>
       </c>
       <c r="Q7">
-        <v>953566</v>
+        <v>814654</v>
       </c>
       <c r="R7">
-        <v>964006</v>
+        <v>819808</v>
       </c>
       <c r="S7">
-        <v>975128</v>
+        <v>824754</v>
       </c>
       <c r="T7">
-        <v>986997</v>
+        <v>830998</v>
       </c>
       <c r="U7">
-        <v>999406</v>
+        <v>836502</v>
       </c>
       <c r="V7" s="13">
-        <v>1012500</v>
+        <v>841698</v>
       </c>
       <c r="W7" s="13">
-        <v>1025280</v>
+        <v>847887</v>
       </c>
       <c r="X7" s="13">
-        <v>1037640</v>
+        <v>853549</v>
       </c>
       <c r="Y7" s="13">
-        <v>1049540</v>
+        <v>859603</v>
       </c>
       <c r="Z7" s="13">
-        <v>1061480</v>
+        <v>866464</v>
       </c>
       <c r="AA7" s="13">
-        <v>1073060</v>
+        <v>873306</v>
       </c>
       <c r="AB7" s="13">
-        <v>1084970</v>
+        <v>881021</v>
       </c>
       <c r="AC7" s="13">
-        <v>1096540</v>
+        <v>888875</v>
       </c>
       <c r="AD7" s="13">
-        <v>1107910</v>
+        <v>896015</v>
       </c>
       <c r="AE7" s="13">
-        <v>1118780</v>
+        <v>903925</v>
       </c>
       <c r="AF7" s="13">
-        <v>1129250</v>
+        <v>912866</v>
       </c>
       <c r="AG7" s="13">
-        <v>1138970</v>
-      </c>
-      <c r="AH7" s="13">
-        <v>1149120</v>
-      </c>
+        <v>922440</v>
+      </c>
+      <c r="AH7" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -883,7 +878,7 @@
   <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D2" sqref="D2:AH2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1008,128 +1003,128 @@
         <v>59000</v>
       </c>
       <c r="D2" s="8">
-        <f>$C$2*(Calculations!D7/Calculations!$C$7)</f>
-        <v>56816.464532194783</v>
+        <f>$C$2*(Calculations!C7/Calculations!$B$7)</f>
+        <v>53577.217418126507</v>
       </c>
       <c r="E2" s="8">
-        <f>$C$2*(Calculations!E7/Calculations!$C$7)</f>
-        <v>58832.246584697867</v>
+        <f>$C$2*(Calculations!D7/Calculations!$B$7)</f>
+        <v>57181.528340619247</v>
       </c>
       <c r="F2" s="8">
-        <f>$C$2*(Calculations!F7/Calculations!$C$7)</f>
-        <v>59841.508145388158</v>
+        <f>$C$2*(Calculations!E7/Calculations!$B$7)</f>
+        <v>58517.96616569344</v>
       </c>
       <c r="G2" s="8">
-        <f>$C$2*(Calculations!G7/Calculations!$C$7)</f>
-        <v>60441.185489060117</v>
+        <f>$C$2*(Calculations!F7/Calculations!$B$7)</f>
+        <v>59414.651073741981</v>
       </c>
       <c r="H2" s="8">
-        <f>$C$2*(Calculations!H7/Calculations!$C$7)</f>
-        <v>60910.319427441813</v>
+        <f>$C$2*(Calculations!G7/Calculations!$B$7)</f>
+        <v>60093.89126434581</v>
       </c>
       <c r="I2" s="8">
-        <f>$C$2*(Calculations!I7/Calculations!$C$7)</f>
-        <v>61332.85519490626</v>
+        <f>$C$2*(Calculations!H7/Calculations!$B$7)</f>
+        <v>60597.026335662697</v>
       </c>
       <c r="J2" s="8">
-        <f>$C$2*(Calculations!J7/Calculations!$C$7)</f>
-        <v>61698.445256440929</v>
+        <f>$C$2*(Calculations!I7/Calculations!$B$7)</f>
+        <v>60929.939532212265</v>
       </c>
       <c r="K2" s="8">
-        <f>$C$2*(Calculations!K7/Calculations!$C$7)</f>
-        <v>62110.496435448993</v>
+        <f>$C$2*(Calculations!J7/Calculations!$B$7)</f>
+        <v>61158.99385217567</v>
       </c>
       <c r="L2" s="8">
-        <f>$C$2*(Calculations!L7/Calculations!$C$7)</f>
-        <v>62645.416026890351</v>
+        <f>$C$2*(Calculations!K7/Calculations!$B$7)</f>
+        <v>61535.992160992158</v>
       </c>
       <c r="M2" s="8">
-        <f>$C$2*(Calculations!M7/Calculations!$C$7)</f>
-        <v>63199.865734083796</v>
+        <f>$C$2*(Calculations!L7/Calculations!$B$7)</f>
+        <v>62153.419062509973</v>
       </c>
       <c r="N2" s="8">
-        <f>$C$2*(Calculations!N7/Calculations!$C$7)</f>
-        <v>63642.822464685501</v>
+        <f>$C$2*(Calculations!M7/Calculations!$B$7)</f>
+        <v>62478.566376293653</v>
       </c>
       <c r="O2" s="8">
-        <f>$C$2*(Calculations!O7/Calculations!$C$7)</f>
-        <v>64182.53892666247</v>
+        <f>$C$2*(Calculations!N7/Calculations!$B$7)</f>
+        <v>62828.893976621257</v>
       </c>
       <c r="P2" s="8">
-        <f>$C$2*(Calculations!P7/Calculations!$C$7)</f>
-        <v>64747.267642146486</v>
+        <f>$C$2*(Calculations!O7/Calculations!$B$7)</f>
+        <v>63235.70072433709</v>
       </c>
       <c r="Q2" s="8">
-        <f>$C$2*(Calculations!Q7/Calculations!$C$7)</f>
-        <v>65344.752130716464</v>
+        <f>$C$2*(Calculations!P7/Calculations!$B$7)</f>
+        <v>63567.907931544294</v>
       </c>
       <c r="R2" s="8">
-        <f>$C$2*(Calculations!R7/Calculations!$C$7)</f>
-        <v>66060.171107740272</v>
+        <f>$C$2*(Calculations!Q7/Calculations!$B$7)</f>
+        <v>63904.115745024836</v>
       </c>
       <c r="S2" s="8">
-        <f>$C$2*(Calculations!S7/Calculations!$C$7)</f>
-        <v>66822.325309125197</v>
+        <f>$C$2*(Calculations!R7/Calculations!$B$7)</f>
+        <v>64308.412308412306</v>
       </c>
       <c r="T2" s="8">
-        <f>$C$2*(Calculations!T7/Calculations!$C$7)</f>
-        <v>67635.668971797189</v>
+        <f>$C$2*(Calculations!S7/Calculations!$B$7)</f>
+        <v>64696.392673665396</v>
       </c>
       <c r="U2" s="8">
-        <f>$C$2*(Calculations!U7/Calculations!$C$7)</f>
-        <v>68486.017064315238</v>
+        <f>$C$2*(Calculations!T7/Calculations!$B$7)</f>
+        <v>65186.192390737844</v>
       </c>
       <c r="V2" s="8">
-        <f>$C$2*(Calculations!V7/Calculations!$C$7)</f>
-        <v>69383.305961360224</v>
+        <f>$C$2*(Calculations!U7/Calculations!$B$7)</f>
+        <v>65617.944095216822</v>
       </c>
       <c r="W2" s="8">
-        <f>$C$2*(Calculations!W7/Calculations!$C$7)</f>
-        <v>70259.077467716954</v>
+        <f>$C$2*(Calculations!V7/Calculations!$B$7)</f>
+        <v>66025.53527553528</v>
       </c>
       <c r="X2" s="8">
-        <f>$C$2*(Calculations!X7/Calculations!$C$7)</f>
-        <v>71106.067750860064</v>
+        <f>$C$2*(Calculations!W7/Calculations!$B$7)</f>
+        <v>66511.020613293338</v>
       </c>
       <c r="Y2" s="8">
-        <f>$C$2*(Calculations!Y7/Calculations!$C$7)</f>
-        <v>71921.535741912099</v>
+        <f>$C$2*(Calculations!X7/Calculations!$B$7)</f>
+        <v>66955.166352893619</v>
       </c>
       <c r="Z2" s="8">
-        <f>$C$2*(Calculations!Z7/Calculations!$C$7)</f>
-        <v>72739.744801841618</v>
+        <f>$C$2*(Calculations!Y7/Calculations!$B$7)</f>
+        <v>67430.061850516402</v>
       </c>
       <c r="AA2" s="8">
-        <f>$C$2*(Calculations!AA7/Calculations!$C$7)</f>
-        <v>73533.284241873771</v>
+        <f>$C$2*(Calculations!Z7/Calculations!$B$7)</f>
+        <v>67968.261059170152</v>
       </c>
       <c r="AB2" s="8">
-        <f>$C$2*(Calculations!AB7/Calculations!$C$7)</f>
-        <v>74349.437500145184</v>
+        <f>$C$2*(Calculations!AA7/Calculations!$B$7)</f>
+        <v>68504.969845878935</v>
       </c>
       <c r="AC2" s="8">
-        <f>$C$2*(Calculations!AC7/Calculations!$C$7)</f>
-        <v>75142.291672957959</v>
+        <f>$C$2*(Calculations!AB7/Calculations!$B$7)</f>
+        <v>69110.159598795974</v>
       </c>
       <c r="AD2" s="8">
-        <f>$C$2*(Calculations!AD7/Calculations!$C$7)</f>
-        <v>75921.440501383317</v>
+        <f>$C$2*(Calculations!AC7/Calculations!$B$7)</f>
+        <v>69726.252964889325</v>
       </c>
       <c r="AE2" s="8">
-        <f>$C$2*(Calculations!AE7/Calculations!$C$7)</f>
-        <v>76666.325968840087</v>
+        <f>$C$2*(Calculations!AD7/Calculations!$B$7)</f>
+        <v>70286.337843156027</v>
       </c>
       <c r="AF2" s="8">
-        <f>$C$2*(Calculations!AF7/Calculations!$C$7)</f>
-        <v>77383.800747522007</v>
+        <f>$C$2*(Calculations!AE7/Calculations!$B$7)</f>
+        <v>70906.824031824042</v>
       </c>
       <c r="AG2" s="8">
-        <f>$C$2*(Calculations!AG7/Calculations!$C$7)</f>
-        <v>78049.880484751062</v>
+        <f>$C$2*(Calculations!AF7/Calculations!$B$7)</f>
+        <v>71608.185221821579</v>
       </c>
       <c r="AH2" s="8">
-        <f>$C$2*(Calculations!AH7/Calculations!$C$7)</f>
-        <v>78745.4267124131</v>
+        <f>$C$2*(Calculations!AG7/Calculations!$B$7)</f>
+        <v>72359.200995564635</v>
       </c>
     </row>
   </sheetData>
@@ -1145,7 +1140,7 @@
   <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="O2" sqref="O2:AH2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1263,135 +1258,135 @@
       </c>
       <c r="B2" s="8">
         <f>C2</f>
-        <v>59000</v>
+        <v>0</v>
       </c>
       <c r="C2" s="8">
-        <f>Calculations!A3</f>
-        <v>59000</v>
+        <f>Calculations!A3-'DRC-BDRC'!C2</f>
+        <v>0</v>
       </c>
       <c r="D2" s="8">
-        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!D1)</f>
-        <v>71636.363636363298</v>
+        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!D1)-'DRC-BDRC'!D2</f>
+        <v>18059.14621823679</v>
       </c>
       <c r="E2" s="8">
-        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!E1)</f>
-        <v>84272.727272730321</v>
+        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!E1)-'DRC-BDRC'!E2</f>
+        <v>27091.198932111074</v>
       </c>
       <c r="F2" s="8">
-        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!F1)</f>
-        <v>96909.090909093618</v>
+        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!F1)-'DRC-BDRC'!F2</f>
+        <v>38391.124743400178</v>
       </c>
       <c r="G2" s="8">
-        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!G1)</f>
-        <v>109545.45454545692</v>
+        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!G1)-'DRC-BDRC'!G2</f>
+        <v>50130.803471714935</v>
       </c>
       <c r="H2" s="8">
-        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!H1)</f>
-        <v>122181.81818182021</v>
+        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!H1)-'DRC-BDRC'!H2</f>
+        <v>62087.926917474404</v>
       </c>
       <c r="I2" s="8">
-        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!I1)</f>
-        <v>134818.18181818351</v>
+        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!I1)-'DRC-BDRC'!I2</f>
+        <v>74221.155482520815</v>
       </c>
       <c r="J2" s="8">
-        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!J1)</f>
-        <v>147454.54545454681</v>
+        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!J1)-'DRC-BDRC'!J2</f>
+        <v>86524.605922334536</v>
       </c>
       <c r="K2" s="8">
-        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!K1)</f>
-        <v>160090.90909091011</v>
+        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!K1)-'DRC-BDRC'!K2</f>
+        <v>98931.915238734437</v>
       </c>
       <c r="L2" s="8">
-        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!L1)</f>
-        <v>172727.2727272734</v>
+        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!L1)-'DRC-BDRC'!L2</f>
+        <v>111191.28056628125</v>
       </c>
       <c r="M2" s="8">
-        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!M1)</f>
-        <v>185363.6363636367</v>
+        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!M1)-'DRC-BDRC'!M2</f>
+        <v>123210.21730112673</v>
       </c>
       <c r="N2" s="8">
-        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!N1)</f>
-        <v>198000</v>
+        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!N1)-'DRC-BDRC'!N2</f>
+        <v>135521.43362370634</v>
       </c>
       <c r="O2" s="8">
-        <f>$N$2*(Calculations!O7/Calculations!$N$7)</f>
-        <v>199679.11879663626</v>
+        <f>$N$2*(Calculations!N7/Calculations!$M$7)-'DRC-BDRC'!O2</f>
+        <v>73452.430620709682</v>
       </c>
       <c r="P2" s="8">
-        <f>$N$2*(Calculations!P7/Calculations!$N$7)</f>
-        <v>201436.05353547315</v>
+        <f>$N$2*(Calculations!O7/Calculations!$M$7)-'DRC-BDRC'!P2</f>
+        <v>73928.023019706088</v>
       </c>
       <c r="Q2" s="8">
-        <f>$N$2*(Calculations!Q7/Calculations!$N$7)</f>
-        <v>203294.89517943861</v>
+        <f>$N$2*(Calculations!P7/Calculations!$M$7)-'DRC-BDRC'!Q2</f>
+        <v>74316.402080591157</v>
       </c>
       <c r="R2" s="8">
-        <f>$N$2*(Calculations!R7/Calculations!$N$7)</f>
-        <v>205520.64432073908</v>
+        <f>$N$2*(Calculations!Q7/Calculations!$M$7)-'DRC-BDRC'!R2</f>
+        <v>74709.458197463275</v>
       </c>
       <c r="S2" s="8">
-        <f>$N$2*(Calculations!S7/Calculations!$N$7)</f>
-        <v>207891.79201705556</v>
+        <f>$N$2*(Calculations!R7/Calculations!$M$7)-'DRC-BDRC'!S2</f>
+        <v>75182.115973095293</v>
       </c>
       <c r="T2" s="8">
-        <f>$N$2*(Calculations!T7/Calculations!$N$7)</f>
-        <v>210422.19590193059</v>
+        <f>$N$2*(Calculations!S7/Calculations!$M$7)-'DRC-BDRC'!T2</f>
+        <v>75635.69869685857</v>
       </c>
       <c r="U2" s="8">
-        <f>$N$2*(Calculations!U7/Calculations!$N$7)</f>
-        <v>213067.72474239013</v>
+        <f>$N$2*(Calculations!T7/Calculations!$M$7)-'DRC-BDRC'!U2</f>
+        <v>76208.317080841167</v>
       </c>
       <c r="V2" s="8">
-        <f>$N$2*(Calculations!V7/Calculations!$N$7)</f>
-        <v>215859.29172095226</v>
+        <f>$N$2*(Calculations!U7/Calculations!$M$7)-'DRC-BDRC'!V2</f>
+        <v>76713.072299521547</v>
       </c>
       <c r="W2" s="8">
-        <f>$N$2*(Calculations!W7/Calculations!$N$7)</f>
-        <v>218583.91566978561</v>
+        <f>$N$2*(Calculations!V7/Calculations!$M$7)-'DRC-BDRC'!W2</f>
+        <v>77189.58176831936</v>
       </c>
       <c r="X2" s="8">
-        <f>$N$2*(Calculations!X7/Calculations!$N$7)</f>
-        <v>221218.99798649768</v>
+        <f>$N$2*(Calculations!W7/Calculations!$M$7)-'DRC-BDRC'!X2</f>
+        <v>77757.156268394378</v>
       </c>
       <c r="Y2" s="8">
-        <f>$N$2*(Calculations!Y7/Calculations!$N$7)</f>
-        <v>223756.01089660072</v>
+        <f>$N$2*(Calculations!X7/Calculations!$M$7)-'DRC-BDRC'!Y2</f>
+        <v>78276.401189936572</v>
       </c>
       <c r="Z2" s="8">
-        <f>$N$2*(Calculations!Z7/Calculations!$N$7)</f>
-        <v>226301.55158119151</v>
+        <f>$N$2*(Calculations!Y7/Calculations!$M$7)-'DRC-BDRC'!Z2</f>
+        <v>78831.59524769288</v>
       </c>
       <c r="AA2" s="8">
-        <f>$N$2*(Calculations!AA7/Calculations!$N$7)</f>
-        <v>228770.34229539265</v>
+        <f>$N$2*(Calculations!Z7/Calculations!$M$7)-'DRC-BDRC'!AA2</f>
+        <v>79460.796838420734</v>
       </c>
       <c r="AB2" s="8">
-        <f>$N$2*(Calculations!AB7/Calculations!$N$7)</f>
-        <v>231309.4871491176</v>
+        <f>$N$2*(Calculations!AA7/Calculations!$M$7)-'DRC-BDRC'!AB2</f>
+        <v>80088.255996525942</v>
       </c>
       <c r="AC2" s="8">
-        <f>$N$2*(Calculations!AC7/Calculations!$N$7)</f>
-        <v>233776.14591969681</v>
+        <f>$N$2*(Calculations!AB7/Calculations!$M$7)-'DRC-BDRC'!AC2</f>
+        <v>80795.775348291776</v>
       </c>
       <c r="AD2" s="8">
-        <f>$N$2*(Calculations!AD7/Calculations!$N$7)</f>
-        <v>236200.16581783726</v>
+        <f>$N$2*(Calculations!AC7/Calculations!$M$7)-'DRC-BDRC'!AD2</f>
+        <v>81516.041970296777</v>
       </c>
       <c r="AE2" s="8">
-        <f>$N$2*(Calculations!AE7/Calculations!$N$7)</f>
-        <v>238517.58853488098</v>
+        <f>$N$2*(Calculations!AD7/Calculations!$M$7)-'DRC-BDRC'!AE2</f>
+        <v>82170.829808483148</v>
       </c>
       <c r="AF2" s="8">
-        <f>$N$2*(Calculations!AF7/Calculations!$N$7)</f>
-        <v>240749.73350704726</v>
+        <f>$N$2*(Calculations!AE7/Calculations!$M$7)-'DRC-BDRC'!AF2</f>
+        <v>82896.232021375909</v>
       </c>
       <c r="AG2" s="8">
-        <f>$N$2*(Calculations!AG7/Calculations!$N$7)</f>
-        <v>242821.98270756842</v>
+        <f>$N$2*(Calculations!AF7/Calculations!$M$7)-'DRC-BDRC'!AG2</f>
+        <v>83716.184130791124</v>
       </c>
       <c r="AH2" s="8">
-        <f>$N$2*(Calculations!AH7/Calculations!$N$7)</f>
-        <v>244985.90548383276</v>
+        <f>$N$2*(Calculations!AG7/Calculations!$M$7)-'DRC-BDRC'!AH2</f>
+        <v>84594.186758633732</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed bug in PADRC
</commit_message>
<xml_diff>
--- a/InputData/elec/DRC/Demand Response Capacity.xlsx
+++ b/InputData/elec/DRC/Demand Response Capacity.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-us\InputData\elec\DRC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\DRC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="180" windowWidth="23955" windowHeight="12270"/>
+    <workbookView xWindow="120" yWindow="180" windowWidth="23955" windowHeight="12270" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -474,26 +474,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="28.59765625" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -501,114 +501,114 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>2019</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B19" s="6"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="5"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="7"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B30" s="6"/>
     </row>
   </sheetData>
@@ -625,22 +625,22 @@
   <dimension ref="A1:AH7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AH6" sqref="AH6:AH7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.9296875" customWidth="1"/>
+    <col min="1" max="1" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>13</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
     </row>
-    <row r="2" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>2019</v>
       </c>
@@ -648,7 +648,7 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>59000</v>
       </c>
@@ -656,12 +656,12 @@
         <v>198000</v>
       </c>
     </row>
-    <row r="5" spans="1:34" s="11" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:34" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -762,7 +762,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -877,16 +877,16 @@
   </sheetPr>
   <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:AH2"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:AH2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.265625" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -990,7 +990,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1139,16 +1139,16 @@
   </sheetPr>
   <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O2" sqref="O2:AH2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2:AH2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1252,7 +1252,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:34" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
@@ -1309,84 +1309,84 @@
         <v>135521.43362370634</v>
       </c>
       <c r="O2" s="8">
-        <f>$N$2*(Calculations!N7/Calculations!$M$7)-'DRC-BDRC'!O2</f>
-        <v>73452.430620709682</v>
+        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!O1)-'DRC-BDRC'!O2</f>
+        <v>147807.46965974203</v>
       </c>
       <c r="P2" s="8">
-        <f>$N$2*(Calculations!O7/Calculations!$M$7)-'DRC-BDRC'!P2</f>
-        <v>73928.023019706088</v>
+        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!P1)-'DRC-BDRC'!P2</f>
+        <v>160037.02654839325</v>
       </c>
       <c r="Q2" s="8">
-        <f>$N$2*(Calculations!P7/Calculations!$M$7)-'DRC-BDRC'!Q2</f>
-        <v>74316.402080591157</v>
+        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!Q1)-'DRC-BDRC'!Q2</f>
+        <v>172341.18297754932</v>
       </c>
       <c r="R2" s="8">
-        <f>$N$2*(Calculations!Q7/Calculations!$M$7)-'DRC-BDRC'!R2</f>
-        <v>74709.458197463275</v>
+        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!R1)-'DRC-BDRC'!R2</f>
+        <v>184641.33880043207</v>
       </c>
       <c r="S2" s="8">
-        <f>$N$2*(Calculations!R7/Calculations!$M$7)-'DRC-BDRC'!S2</f>
-        <v>75182.115973095293</v>
+        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!S1)-'DRC-BDRC'!S2</f>
+        <v>196873.4058734079</v>
       </c>
       <c r="T2" s="8">
-        <f>$N$2*(Calculations!S7/Calculations!$M$7)-'DRC-BDRC'!T2</f>
-        <v>75635.69869685857</v>
+        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!T1)-'DRC-BDRC'!T2</f>
+        <v>209121.78914451812</v>
       </c>
       <c r="U2" s="8">
-        <f>$N$2*(Calculations!T7/Calculations!$M$7)-'DRC-BDRC'!U2</f>
-        <v>76208.317080841167</v>
+        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!U1)-'DRC-BDRC'!U2</f>
+        <v>221268.35306380896</v>
       </c>
       <c r="V2" s="8">
-        <f>$N$2*(Calculations!U7/Calculations!$M$7)-'DRC-BDRC'!V2</f>
-        <v>76713.072299521547</v>
+        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!V1)-'DRC-BDRC'!V2</f>
+        <v>233472.9649956933</v>
       </c>
       <c r="W2" s="8">
-        <f>$N$2*(Calculations!V7/Calculations!$M$7)-'DRC-BDRC'!W2</f>
-        <v>77189.58176831936</v>
+        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!W1)-'DRC-BDRC'!W2</f>
+        <v>245701.73745173812</v>
       </c>
       <c r="X2" s="8">
-        <f>$N$2*(Calculations!W7/Calculations!$M$7)-'DRC-BDRC'!X2</f>
-        <v>77757.156268394378</v>
+        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!X1)-'DRC-BDRC'!X2</f>
+        <v>257852.61575034336</v>
       </c>
       <c r="Y2" s="8">
-        <f>$N$2*(Calculations!X7/Calculations!$M$7)-'DRC-BDRC'!Y2</f>
-        <v>78276.401189936572</v>
+        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!Y1)-'DRC-BDRC'!Y2</f>
+        <v>270044.83364710637</v>
       </c>
       <c r="Z2" s="8">
-        <f>$N$2*(Calculations!Y7/Calculations!$M$7)-'DRC-BDRC'!Z2</f>
-        <v>78831.59524769288</v>
+        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!Z1)-'DRC-BDRC'!Z2</f>
+        <v>282206.30178584688</v>
       </c>
       <c r="AA2" s="8">
-        <f>$N$2*(Calculations!Z7/Calculations!$M$7)-'DRC-BDRC'!AA2</f>
-        <v>79460.796838420734</v>
+        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!AA1)-'DRC-BDRC'!AA2</f>
+        <v>294304.4662135602</v>
       </c>
       <c r="AB2" s="8">
-        <f>$N$2*(Calculations!AA7/Calculations!$M$7)-'DRC-BDRC'!AB2</f>
-        <v>80088.255996525942</v>
+        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!AB1)-'DRC-BDRC'!AB2</f>
+        <v>306404.12106321467</v>
       </c>
       <c r="AC2" s="8">
-        <f>$N$2*(Calculations!AB7/Calculations!$M$7)-'DRC-BDRC'!AC2</f>
-        <v>80795.775348291776</v>
+        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!AC1)-'DRC-BDRC'!AC2</f>
+        <v>318435.29494666093</v>
       </c>
       <c r="AD2" s="8">
-        <f>$N$2*(Calculations!AC7/Calculations!$M$7)-'DRC-BDRC'!AD2</f>
-        <v>81516.041970296777</v>
+        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!AD1)-'DRC-BDRC'!AD2</f>
+        <v>330455.56521693087</v>
       </c>
       <c r="AE2" s="8">
-        <f>$N$2*(Calculations!AD7/Calculations!$M$7)-'DRC-BDRC'!AE2</f>
-        <v>82170.829808483148</v>
+        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!AE1)-'DRC-BDRC'!AE2</f>
+        <v>342531.8439750275</v>
       </c>
       <c r="AF2" s="8">
-        <f>$N$2*(Calculations!AE7/Calculations!$M$7)-'DRC-BDRC'!AF2</f>
-        <v>82896.232021375909</v>
+        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!AF1)-'DRC-BDRC'!AF2</f>
+        <v>354547.7214227228</v>
       </c>
       <c r="AG2" s="8">
-        <f>$N$2*(Calculations!AF7/Calculations!$M$7)-'DRC-BDRC'!AG2</f>
-        <v>83716.184130791124</v>
+        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!AG1)-'DRC-BDRC'!AG2</f>
+        <v>366482.72386908851</v>
       </c>
       <c r="AH2" s="8">
-        <f>$N$2*(Calculations!AG7/Calculations!$M$7)-'DRC-BDRC'!AH2</f>
-        <v>84594.186758633732</v>
+        <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!AH1)-'DRC-BDRC'!AH2</f>
+        <v>378368.07173170877</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add RAF Resource Availability Factor, set BAU demand response to zero, and tweak costs used in reliability-based capacity construction (#232)
</commit_message>
<xml_diff>
--- a/InputData/elec/DRC/Demand Response Capacity.xlsx
+++ b/InputData/elec/DRC/Demand Response Capacity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\elec\DRC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B483B22-3772-4B05-9D90-3CB6740AB686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F517F58C-6EC1-48FC-BFC8-364359C4C4B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17070" yWindow="3840" windowWidth="24000" windowHeight="17205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14445" yWindow="2265" windowWidth="26250" windowHeight="19680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>Year</t>
   </si>
@@ -83,27 +83,6 @@
     <t>2019 Capacity and 2030 Projection</t>
   </si>
   <si>
-    <t>Time (Year)</t>
-  </si>
-  <si>
-    <t>Peak Demand - EPS Output</t>
-  </si>
-  <si>
-    <t>To estimate BAU DR Capacity, we scale Brattle's 2019 estimate of demand response potential by</t>
-  </si>
-  <si>
-    <t>the growth in peak demand (EPS model output).</t>
-  </si>
-  <si>
-    <t>We use a Brattle analysis to estimate the potential in 2030, and scale the potential between 2019 and 2030 linearly.</t>
-  </si>
-  <si>
-    <t>We then scale the potential from 2030 to 2050 by the growth in peak demand (EPS model output).</t>
-  </si>
-  <si>
-    <t>Peak Power Demand after Storage and DR[summer] : MostRecentRun</t>
-  </si>
-  <si>
     <t>DRC Hours of Demand Response Available per Day</t>
   </si>
   <si>
@@ -153,6 +132,9 @@
   </si>
   <si>
     <t>in every day of the year in the EPS model.</t>
+  </si>
+  <si>
+    <t>We use a Brattle analysis to estimate the potential in 2030, and scale the potential between 2019 and 2050 linearly.</t>
   </si>
 </sst>
 </file>
@@ -225,7 +207,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -245,7 +227,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -592,7 +573,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
   </sheetViews>
@@ -613,7 +594,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -651,32 +632,32 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" s="11" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -695,88 +676,66 @@
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
+      <c r="A22" s="4" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>17</v>
-      </c>
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="A24" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="16"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
+      <c r="A25" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="6"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>19</v>
-      </c>
+      <c r="A26" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="6"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B27" s="6"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
+      <c r="A28" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="B28" s="6"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="B29" s="17"/>
+      <c r="A29" s="6"/>
+      <c r="B29" s="5"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B30" s="6"/>
+      <c r="A30" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="7"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>34</v>
+      <c r="A31" s="17" t="s">
+        <v>31</v>
       </c>
       <c r="B31" s="6"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="A32" s="6"/>
       <c r="B32" s="6"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
-        <v>36</v>
-      </c>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="6"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
-      <c r="B34" s="5"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B35" s="7"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="B36" s="6"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B38" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -790,7 +749,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AH7"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -799,14 +758,14 @@
     <col min="1" max="1" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>13</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
     </row>
-    <row r="2" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>2019</v>
       </c>
@@ -814,221 +773,13 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>59000</v>
       </c>
       <c r="B3">
         <v>198000</v>
       </c>
-    </row>
-    <row r="5" spans="1:34" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6">
-        <v>2019</v>
-      </c>
-      <c r="C6">
-        <v>2020</v>
-      </c>
-      <c r="D6">
-        <v>2021</v>
-      </c>
-      <c r="E6">
-        <v>2022</v>
-      </c>
-      <c r="F6">
-        <v>2023</v>
-      </c>
-      <c r="G6">
-        <v>2024</v>
-      </c>
-      <c r="H6">
-        <v>2025</v>
-      </c>
-      <c r="I6">
-        <v>2026</v>
-      </c>
-      <c r="J6">
-        <v>2027</v>
-      </c>
-      <c r="K6">
-        <v>2028</v>
-      </c>
-      <c r="L6">
-        <v>2029</v>
-      </c>
-      <c r="M6">
-        <v>2030</v>
-      </c>
-      <c r="N6">
-        <v>2031</v>
-      </c>
-      <c r="O6">
-        <v>2032</v>
-      </c>
-      <c r="P6">
-        <v>2033</v>
-      </c>
-      <c r="Q6">
-        <v>2034</v>
-      </c>
-      <c r="R6">
-        <v>2035</v>
-      </c>
-      <c r="S6">
-        <v>2036</v>
-      </c>
-      <c r="T6">
-        <v>2037</v>
-      </c>
-      <c r="U6">
-        <v>2038</v>
-      </c>
-      <c r="V6">
-        <v>2039</v>
-      </c>
-      <c r="W6">
-        <v>2040</v>
-      </c>
-      <c r="X6">
-        <v>2041</v>
-      </c>
-      <c r="Y6">
-        <v>2042</v>
-      </c>
-      <c r="Z6">
-        <v>2043</v>
-      </c>
-      <c r="AA6">
-        <v>2044</v>
-      </c>
-      <c r="AB6">
-        <v>2045</v>
-      </c>
-      <c r="AC6">
-        <v>2046</v>
-      </c>
-      <c r="AD6">
-        <v>2047</v>
-      </c>
-      <c r="AE6">
-        <v>2048</v>
-      </c>
-      <c r="AF6">
-        <v>2049</v>
-      </c>
-      <c r="AG6">
-        <v>2050</v>
-      </c>
-    </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7">
-        <v>752136</v>
-      </c>
-      <c r="C7">
-        <v>683006</v>
-      </c>
-      <c r="D7">
-        <v>728954</v>
-      </c>
-      <c r="E7">
-        <v>745991</v>
-      </c>
-      <c r="F7">
-        <v>757422</v>
-      </c>
-      <c r="G7">
-        <v>766081</v>
-      </c>
-      <c r="H7">
-        <v>772495</v>
-      </c>
-      <c r="I7">
-        <v>776739</v>
-      </c>
-      <c r="J7">
-        <v>779659</v>
-      </c>
-      <c r="K7">
-        <v>784465</v>
-      </c>
-      <c r="L7">
-        <v>792336</v>
-      </c>
-      <c r="M7">
-        <v>796481</v>
-      </c>
-      <c r="N7">
-        <v>800947</v>
-      </c>
-      <c r="O7">
-        <v>806133</v>
-      </c>
-      <c r="P7">
-        <v>810368</v>
-      </c>
-      <c r="Q7">
-        <v>814654</v>
-      </c>
-      <c r="R7">
-        <v>819808</v>
-      </c>
-      <c r="S7">
-        <v>824754</v>
-      </c>
-      <c r="T7">
-        <v>830998</v>
-      </c>
-      <c r="U7">
-        <v>836502</v>
-      </c>
-      <c r="V7" s="13">
-        <v>841698</v>
-      </c>
-      <c r="W7" s="13">
-        <v>847887</v>
-      </c>
-      <c r="X7" s="13">
-        <v>853549</v>
-      </c>
-      <c r="Y7" s="13">
-        <v>859603</v>
-      </c>
-      <c r="Z7" s="13">
-        <v>866464</v>
-      </c>
-      <c r="AA7" s="13">
-        <v>873306</v>
-      </c>
-      <c r="AB7" s="13">
-        <v>881021</v>
-      </c>
-      <c r="AC7" s="13">
-        <v>888875</v>
-      </c>
-      <c r="AD7" s="13">
-        <v>896015</v>
-      </c>
-      <c r="AE7" s="13">
-        <v>903925</v>
-      </c>
-      <c r="AF7" s="13">
-        <v>912866</v>
-      </c>
-      <c r="AG7" s="13">
-        <v>922440</v>
-      </c>
-      <c r="AH7" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1159,136 +910,103 @@
         <v>2</v>
       </c>
       <c r="B2" s="8">
-        <f>C2</f>
-        <v>59000</v>
+        <v>0</v>
       </c>
       <c r="C2" s="8">
-        <f>Calculations!A3</f>
-        <v>59000</v>
+        <v>0</v>
       </c>
       <c r="D2" s="8">
-        <f>$C$2*(Calculations!C7/Calculations!$B$7)</f>
-        <v>53577.217418126507</v>
+        <v>0</v>
       </c>
       <c r="E2" s="8">
-        <f>$C$2*(Calculations!D7/Calculations!$B$7)</f>
-        <v>57181.528340619247</v>
+        <v>0</v>
       </c>
       <c r="F2" s="8">
-        <f>$C$2*(Calculations!E7/Calculations!$B$7)</f>
-        <v>58517.96616569344</v>
+        <v>0</v>
       </c>
       <c r="G2" s="8">
-        <f>$C$2*(Calculations!F7/Calculations!$B$7)</f>
-        <v>59414.651073741981</v>
+        <v>0</v>
       </c>
       <c r="H2" s="8">
-        <f>$C$2*(Calculations!G7/Calculations!$B$7)</f>
-        <v>60093.89126434581</v>
+        <v>0</v>
       </c>
       <c r="I2" s="8">
-        <f>$C$2*(Calculations!H7/Calculations!$B$7)</f>
-        <v>60597.026335662697</v>
+        <v>0</v>
       </c>
       <c r="J2" s="8">
-        <f>$C$2*(Calculations!I7/Calculations!$B$7)</f>
-        <v>60929.939532212265</v>
+        <v>0</v>
       </c>
       <c r="K2" s="8">
-        <f>$C$2*(Calculations!J7/Calculations!$B$7)</f>
-        <v>61158.99385217567</v>
+        <v>0</v>
       </c>
       <c r="L2" s="8">
-        <f>$C$2*(Calculations!K7/Calculations!$B$7)</f>
-        <v>61535.992160992158</v>
+        <v>0</v>
       </c>
       <c r="M2" s="8">
-        <f>$C$2*(Calculations!L7/Calculations!$B$7)</f>
-        <v>62153.419062509973</v>
+        <v>0</v>
       </c>
       <c r="N2" s="8">
-        <f>$C$2*(Calculations!M7/Calculations!$B$7)</f>
-        <v>62478.566376293653</v>
+        <v>0</v>
       </c>
       <c r="O2" s="8">
-        <f>$C$2*(Calculations!N7/Calculations!$B$7)</f>
-        <v>62828.893976621257</v>
+        <v>0</v>
       </c>
       <c r="P2" s="8">
-        <f>$C$2*(Calculations!O7/Calculations!$B$7)</f>
-        <v>63235.70072433709</v>
+        <v>0</v>
       </c>
       <c r="Q2" s="8">
-        <f>$C$2*(Calculations!P7/Calculations!$B$7)</f>
-        <v>63567.907931544294</v>
+        <v>0</v>
       </c>
       <c r="R2" s="8">
-        <f>$C$2*(Calculations!Q7/Calculations!$B$7)</f>
-        <v>63904.115745024836</v>
+        <v>0</v>
       </c>
       <c r="S2" s="8">
-        <f>$C$2*(Calculations!R7/Calculations!$B$7)</f>
-        <v>64308.412308412306</v>
+        <v>0</v>
       </c>
       <c r="T2" s="8">
-        <f>$C$2*(Calculations!S7/Calculations!$B$7)</f>
-        <v>64696.392673665396</v>
+        <v>0</v>
       </c>
       <c r="U2" s="8">
-        <f>$C$2*(Calculations!T7/Calculations!$B$7)</f>
-        <v>65186.192390737844</v>
+        <v>0</v>
       </c>
       <c r="V2" s="8">
-        <f>$C$2*(Calculations!U7/Calculations!$B$7)</f>
-        <v>65617.944095216822</v>
+        <v>0</v>
       </c>
       <c r="W2" s="8">
-        <f>$C$2*(Calculations!V7/Calculations!$B$7)</f>
-        <v>66025.53527553528</v>
+        <v>0</v>
       </c>
       <c r="X2" s="8">
-        <f>$C$2*(Calculations!W7/Calculations!$B$7)</f>
-        <v>66511.020613293338</v>
+        <v>0</v>
       </c>
       <c r="Y2" s="8">
-        <f>$C$2*(Calculations!X7/Calculations!$B$7)</f>
-        <v>66955.166352893619</v>
+        <v>0</v>
       </c>
       <c r="Z2" s="8">
-        <f>$C$2*(Calculations!Y7/Calculations!$B$7)</f>
-        <v>67430.061850516402</v>
+        <v>0</v>
       </c>
       <c r="AA2" s="8">
-        <f>$C$2*(Calculations!Z7/Calculations!$B$7)</f>
-        <v>67968.261059170152</v>
+        <v>0</v>
       </c>
       <c r="AB2" s="8">
-        <f>$C$2*(Calculations!AA7/Calculations!$B$7)</f>
-        <v>68504.969845878935</v>
+        <v>0</v>
       </c>
       <c r="AC2" s="8">
-        <f>$C$2*(Calculations!AB7/Calculations!$B$7)</f>
-        <v>69110.159598795974</v>
+        <v>0</v>
       </c>
       <c r="AD2" s="8">
-        <f>$C$2*(Calculations!AC7/Calculations!$B$7)</f>
-        <v>69726.252964889325</v>
+        <v>0</v>
       </c>
       <c r="AE2" s="8">
-        <f>$C$2*(Calculations!AD7/Calculations!$B$7)</f>
-        <v>70286.337843156027</v>
+        <v>0</v>
       </c>
       <c r="AF2" s="8">
-        <f>$C$2*(Calculations!AE7/Calculations!$B$7)</f>
-        <v>70906.824031824042</v>
+        <v>0</v>
       </c>
       <c r="AG2" s="8">
-        <f>$C$2*(Calculations!AF7/Calculations!$B$7)</f>
-        <v>71608.185221821579</v>
+        <v>0</v>
       </c>
       <c r="AH2" s="8">
-        <f>$C$2*(Calculations!AG7/Calculations!$B$7)</f>
-        <v>72359.200995564635</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1303,9 +1021,7 @@
   </sheetPr>
   <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2:AH2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1422,135 +1138,135 @@
       </c>
       <c r="B2" s="8">
         <f>C2</f>
-        <v>0</v>
+        <v>59000</v>
       </c>
       <c r="C2" s="8">
         <f>Calculations!A3-'DRC-BDRC'!C2</f>
-        <v>0</v>
+        <v>59000</v>
       </c>
       <c r="D2" s="8">
         <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!D1)-'DRC-BDRC'!D2</f>
-        <v>18059.14621823679</v>
+        <v>71636.363636363298</v>
       </c>
       <c r="E2" s="8">
         <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!E1)-'DRC-BDRC'!E2</f>
-        <v>27091.198932111074</v>
+        <v>84272.727272730321</v>
       </c>
       <c r="F2" s="8">
         <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!F1)-'DRC-BDRC'!F2</f>
-        <v>38391.124743400178</v>
+        <v>96909.090909093618</v>
       </c>
       <c r="G2" s="8">
         <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!G1)-'DRC-BDRC'!G2</f>
-        <v>50130.803471714935</v>
+        <v>109545.45454545692</v>
       </c>
       <c r="H2" s="8">
         <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!H1)-'DRC-BDRC'!H2</f>
-        <v>62087.926917474404</v>
+        <v>122181.81818182021</v>
       </c>
       <c r="I2" s="8">
         <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!I1)-'DRC-BDRC'!I2</f>
-        <v>74221.155482520815</v>
+        <v>134818.18181818351</v>
       </c>
       <c r="J2" s="8">
         <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!J1)-'DRC-BDRC'!J2</f>
-        <v>86524.605922334536</v>
+        <v>147454.54545454681</v>
       </c>
       <c r="K2" s="8">
         <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!K1)-'DRC-BDRC'!K2</f>
-        <v>98931.915238734437</v>
+        <v>160090.90909091011</v>
       </c>
       <c r="L2" s="8">
         <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!L1)-'DRC-BDRC'!L2</f>
-        <v>111191.28056628125</v>
+        <v>172727.2727272734</v>
       </c>
       <c r="M2" s="8">
         <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!M1)-'DRC-BDRC'!M2</f>
-        <v>123210.21730112673</v>
+        <v>185363.6363636367</v>
       </c>
       <c r="N2" s="8">
         <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!N1)-'DRC-BDRC'!N2</f>
-        <v>135521.43362370634</v>
+        <v>198000</v>
       </c>
       <c r="O2" s="8">
         <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!O1)-'DRC-BDRC'!O2</f>
-        <v>147807.46965974203</v>
+        <v>210636.3636363633</v>
       </c>
       <c r="P2" s="8">
         <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!P1)-'DRC-BDRC'!P2</f>
-        <v>160037.02654839325</v>
+        <v>223272.72727273032</v>
       </c>
       <c r="Q2" s="8">
         <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!Q1)-'DRC-BDRC'!Q2</f>
-        <v>172341.18297754932</v>
+        <v>235909.09090909362</v>
       </c>
       <c r="R2" s="8">
         <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!R1)-'DRC-BDRC'!R2</f>
-        <v>184641.33880043207</v>
+        <v>248545.45454545692</v>
       </c>
       <c r="S2" s="8">
         <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!S1)-'DRC-BDRC'!S2</f>
-        <v>196873.4058734079</v>
+        <v>261181.81818182021</v>
       </c>
       <c r="T2" s="8">
         <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!T1)-'DRC-BDRC'!T2</f>
-        <v>209121.78914451812</v>
+        <v>273818.18181818351</v>
       </c>
       <c r="U2" s="8">
         <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!U1)-'DRC-BDRC'!U2</f>
-        <v>221268.35306380896</v>
+        <v>286454.54545454681</v>
       </c>
       <c r="V2" s="8">
         <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!V1)-'DRC-BDRC'!V2</f>
-        <v>233472.9649956933</v>
+        <v>299090.90909091011</v>
       </c>
       <c r="W2" s="8">
         <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!W1)-'DRC-BDRC'!W2</f>
-        <v>245701.73745173812</v>
+        <v>311727.2727272734</v>
       </c>
       <c r="X2" s="8">
         <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!X1)-'DRC-BDRC'!X2</f>
-        <v>257852.61575034336</v>
+        <v>324363.6363636367</v>
       </c>
       <c r="Y2" s="8">
         <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!Y1)-'DRC-BDRC'!Y2</f>
-        <v>270044.83364710637</v>
+        <v>337000</v>
       </c>
       <c r="Z2" s="8">
         <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!Z1)-'DRC-BDRC'!Z2</f>
-        <v>282206.30178584688</v>
+        <v>349636.3636363633</v>
       </c>
       <c r="AA2" s="8">
         <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!AA1)-'DRC-BDRC'!AA2</f>
-        <v>294304.4662135602</v>
+        <v>362272.72727273032</v>
       </c>
       <c r="AB2" s="8">
         <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!AB1)-'DRC-BDRC'!AB2</f>
-        <v>306404.12106321467</v>
+        <v>374909.09090909362</v>
       </c>
       <c r="AC2" s="8">
         <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!AC1)-'DRC-BDRC'!AC2</f>
-        <v>318435.29494666093</v>
+        <v>387545.45454545692</v>
       </c>
       <c r="AD2" s="8">
         <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!AD1)-'DRC-BDRC'!AD2</f>
-        <v>330455.56521693087</v>
+        <v>400181.81818182021</v>
       </c>
       <c r="AE2" s="8">
         <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!AE1)-'DRC-BDRC'!AE2</f>
-        <v>342531.8439750275</v>
+        <v>412818.18181818351</v>
       </c>
       <c r="AF2" s="8">
         <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!AF1)-'DRC-BDRC'!AF2</f>
-        <v>354547.7214227228</v>
+        <v>425454.54545454681</v>
       </c>
       <c r="AG2" s="8">
         <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!AG1)-'DRC-BDRC'!AG2</f>
-        <v>366482.72386908851</v>
+        <v>438090.90909091011</v>
       </c>
       <c r="AH2" s="8">
         <f>TREND(Calculations!$A$3:$B$3,Calculations!$A$2:$B$2,'DRC-PADRC'!AH1)-'DRC-BDRC'!AH2</f>
-        <v>378368.07173170877</v>
+        <v>450727.2727272734</v>
       </c>
     </row>
   </sheetData>
@@ -1574,16 +1290,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>23</v>
+      <c r="A1" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B2" s="8">
         <v>4</v>

</xml_diff>

<commit_message>
Implements new cost-effectiveness based grid battery capacity expansion, clean up code, fix data error with demand response capacity.
</commit_message>
<xml_diff>
--- a/InputData/elec/DRC/Demand Response Capacity.xlsx
+++ b/InputData/elec/DRC/Demand Response Capacity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\elec\DRC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\DRC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1680B8F-DE4F-472C-A87D-2F994043E621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E14643-8DF8-47DF-923D-41404FE63C2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25530" yWindow="180" windowWidth="31110" windowHeight="20640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="26940" windowHeight="20235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -217,22 +217,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -256,9 +253,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -296,9 +293,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -331,26 +328,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -383,26 +363,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -609,7 +572,7 @@
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>14</v>
       </c>
     </row>
@@ -639,7 +602,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="7" t="s">
         <v>22</v>
       </c>
     </row>
@@ -674,38 +637,32 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="A21" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="A22" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+      <c r="A23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-    </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+      <c r="A25" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="5"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
+      <c r="A26" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="5"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+      <c r="A27" t="s">
         <v>37</v>
       </c>
     </row>
@@ -723,7 +680,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -731,17 +690,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-    </row>
-    <row r="2" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>2019</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2">
         <v>2030</v>
       </c>
     </row>
@@ -754,11 +713,11 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -808,7 +767,9 @@
   </sheetPr>
   <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -923,104 +884,137 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="6">
-        <v>0</v>
-      </c>
-      <c r="C2" s="6">
-        <v>0</v>
-      </c>
-      <c r="D2" s="6">
-        <v>0</v>
-      </c>
-      <c r="E2" s="6">
-        <v>0</v>
-      </c>
-      <c r="F2" s="6">
-        <v>0</v>
-      </c>
-      <c r="G2" s="6">
-        <v>0</v>
-      </c>
-      <c r="H2" s="6">
-        <v>0</v>
-      </c>
-      <c r="I2" s="6">
-        <v>0</v>
-      </c>
-      <c r="J2" s="6">
-        <v>0</v>
-      </c>
-      <c r="K2" s="6">
-        <v>0</v>
-      </c>
-      <c r="L2" s="6">
-        <v>0</v>
-      </c>
-      <c r="M2" s="6">
-        <v>0</v>
-      </c>
-      <c r="N2" s="6">
-        <v>0</v>
-      </c>
-      <c r="O2" s="6">
-        <v>0</v>
-      </c>
-      <c r="P2" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="6">
-        <v>0</v>
-      </c>
-      <c r="R2" s="6">
-        <v>0</v>
-      </c>
-      <c r="S2" s="6">
-        <v>0</v>
-      </c>
-      <c r="T2" s="6">
-        <v>0</v>
-      </c>
-      <c r="U2" s="6">
-        <v>0</v>
-      </c>
-      <c r="V2" s="6">
-        <v>0</v>
-      </c>
-      <c r="W2" s="6">
-        <v>0</v>
-      </c>
-      <c r="X2" s="6">
-        <v>0</v>
-      </c>
-      <c r="Y2" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z2" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA2" s="6">
-        <v>0</v>
-      </c>
-      <c r="AB2" s="6">
-        <v>0</v>
-      </c>
-      <c r="AC2" s="6">
-        <v>0</v>
-      </c>
-      <c r="AD2" s="6">
-        <v>0</v>
-      </c>
-      <c r="AE2" s="6">
-        <v>0</v>
-      </c>
-      <c r="AF2" s="6">
-        <v>0</v>
-      </c>
-      <c r="AG2" s="6">
-        <v>0</v>
-      </c>
-      <c r="AH2" s="6">
-        <v>0</v>
+      <c r="B2" s="4">
+        <f>'Data and Calculations'!A3</f>
+        <v>59000</v>
+      </c>
+      <c r="C2" s="4">
+        <f>B2</f>
+        <v>59000</v>
+      </c>
+      <c r="D2" s="4">
+        <f t="shared" ref="D2:AH2" si="0">C2</f>
+        <v>59000</v>
+      </c>
+      <c r="E2" s="4">
+        <f t="shared" si="0"/>
+        <v>59000</v>
+      </c>
+      <c r="F2" s="4">
+        <f t="shared" si="0"/>
+        <v>59000</v>
+      </c>
+      <c r="G2" s="4">
+        <f t="shared" si="0"/>
+        <v>59000</v>
+      </c>
+      <c r="H2" s="4">
+        <f t="shared" si="0"/>
+        <v>59000</v>
+      </c>
+      <c r="I2" s="4">
+        <f t="shared" si="0"/>
+        <v>59000</v>
+      </c>
+      <c r="J2" s="4">
+        <f t="shared" si="0"/>
+        <v>59000</v>
+      </c>
+      <c r="K2" s="4">
+        <f t="shared" si="0"/>
+        <v>59000</v>
+      </c>
+      <c r="L2" s="4">
+        <f t="shared" si="0"/>
+        <v>59000</v>
+      </c>
+      <c r="M2" s="4">
+        <f t="shared" si="0"/>
+        <v>59000</v>
+      </c>
+      <c r="N2" s="4">
+        <f t="shared" si="0"/>
+        <v>59000</v>
+      </c>
+      <c r="O2" s="4">
+        <f t="shared" si="0"/>
+        <v>59000</v>
+      </c>
+      <c r="P2" s="4">
+        <f t="shared" si="0"/>
+        <v>59000</v>
+      </c>
+      <c r="Q2" s="4">
+        <f t="shared" si="0"/>
+        <v>59000</v>
+      </c>
+      <c r="R2" s="4">
+        <f t="shared" si="0"/>
+        <v>59000</v>
+      </c>
+      <c r="S2" s="4">
+        <f t="shared" si="0"/>
+        <v>59000</v>
+      </c>
+      <c r="T2" s="4">
+        <f t="shared" si="0"/>
+        <v>59000</v>
+      </c>
+      <c r="U2" s="4">
+        <f t="shared" si="0"/>
+        <v>59000</v>
+      </c>
+      <c r="V2" s="4">
+        <f t="shared" si="0"/>
+        <v>59000</v>
+      </c>
+      <c r="W2" s="4">
+        <f t="shared" si="0"/>
+        <v>59000</v>
+      </c>
+      <c r="X2" s="4">
+        <f t="shared" si="0"/>
+        <v>59000</v>
+      </c>
+      <c r="Y2" s="4">
+        <f t="shared" si="0"/>
+        <v>59000</v>
+      </c>
+      <c r="Z2" s="4">
+        <f t="shared" si="0"/>
+        <v>59000</v>
+      </c>
+      <c r="AA2" s="4">
+        <f t="shared" si="0"/>
+        <v>59000</v>
+      </c>
+      <c r="AB2" s="4">
+        <f t="shared" si="0"/>
+        <v>59000</v>
+      </c>
+      <c r="AC2" s="4">
+        <f t="shared" si="0"/>
+        <v>59000</v>
+      </c>
+      <c r="AD2" s="4">
+        <f t="shared" si="0"/>
+        <v>59000</v>
+      </c>
+      <c r="AE2" s="4">
+        <f t="shared" si="0"/>
+        <v>59000</v>
+      </c>
+      <c r="AF2" s="4">
+        <f t="shared" si="0"/>
+        <v>59000</v>
+      </c>
+      <c r="AG2" s="4">
+        <f t="shared" si="0"/>
+        <v>59000</v>
+      </c>
+      <c r="AH2" s="4">
+        <f t="shared" si="0"/>
+        <v>59000</v>
       </c>
     </row>
   </sheetData>
@@ -1035,7 +1029,9 @@
   </sheetPr>
   <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1147,140 +1143,140 @@
       </c>
     </row>
     <row r="2" spans="1:34" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="4">
         <f>C2</f>
-        <v>59000</v>
-      </c>
-      <c r="C2" s="6">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4">
         <f>'Data and Calculations'!A3-'DRC-BDRC'!C2</f>
-        <v>59000</v>
-      </c>
-      <c r="D2" s="6">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4">
         <f>TREND('Data and Calculations'!$A$3:$B$3,'Data and Calculations'!$A$2:$B$2,'DRC-PADRC'!D1)-'DRC-BDRC'!D2</f>
-        <v>71636.363636363298</v>
-      </c>
-      <c r="E2" s="6">
+        <v>12636.363636363298</v>
+      </c>
+      <c r="E2" s="4">
         <f>TREND('Data and Calculations'!$A$3:$B$3,'Data and Calculations'!$A$2:$B$2,'DRC-PADRC'!E1)-'DRC-BDRC'!E2</f>
-        <v>84272.727272730321</v>
-      </c>
-      <c r="F2" s="6">
+        <v>25272.727272730321</v>
+      </c>
+      <c r="F2" s="4">
         <f>TREND('Data and Calculations'!$A$3:$B$3,'Data and Calculations'!$A$2:$B$2,'DRC-PADRC'!F1)-'DRC-BDRC'!F2</f>
-        <v>96909.090909093618</v>
-      </c>
-      <c r="G2" s="6">
+        <v>37909.090909093618</v>
+      </c>
+      <c r="G2" s="4">
         <f>TREND('Data and Calculations'!$A$3:$B$3,'Data and Calculations'!$A$2:$B$2,'DRC-PADRC'!G1)-'DRC-BDRC'!G2</f>
-        <v>109545.45454545692</v>
-      </c>
-      <c r="H2" s="6">
+        <v>50545.454545456916</v>
+      </c>
+      <c r="H2" s="4">
         <f>TREND('Data and Calculations'!$A$3:$B$3,'Data and Calculations'!$A$2:$B$2,'DRC-PADRC'!H1)-'DRC-BDRC'!H2</f>
-        <v>122181.81818182021</v>
-      </c>
-      <c r="I2" s="6">
+        <v>63181.818181820214</v>
+      </c>
+      <c r="I2" s="4">
         <f>TREND('Data and Calculations'!$A$3:$B$3,'Data and Calculations'!$A$2:$B$2,'DRC-PADRC'!I1)-'DRC-BDRC'!I2</f>
-        <v>134818.18181818351</v>
-      </c>
-      <c r="J2" s="6">
+        <v>75818.181818183511</v>
+      </c>
+      <c r="J2" s="4">
         <f>TREND('Data and Calculations'!$A$3:$B$3,'Data and Calculations'!$A$2:$B$2,'DRC-PADRC'!J1)-'DRC-BDRC'!J2</f>
-        <v>147454.54545454681</v>
-      </c>
-      <c r="K2" s="6">
+        <v>88454.545454546809</v>
+      </c>
+      <c r="K2" s="4">
         <f>TREND('Data and Calculations'!$A$3:$B$3,'Data and Calculations'!$A$2:$B$2,'DRC-PADRC'!K1)-'DRC-BDRC'!K2</f>
-        <v>160090.90909091011</v>
-      </c>
-      <c r="L2" s="6">
+        <v>101090.90909091011</v>
+      </c>
+      <c r="L2" s="4">
         <f>TREND('Data and Calculations'!$A$3:$B$3,'Data and Calculations'!$A$2:$B$2,'DRC-PADRC'!L1)-'DRC-BDRC'!L2</f>
-        <v>172727.2727272734</v>
-      </c>
-      <c r="M2" s="6">
+        <v>113727.2727272734</v>
+      </c>
+      <c r="M2" s="4">
         <f>TREND('Data and Calculations'!$A$3:$B$3,'Data and Calculations'!$A$2:$B$2,'DRC-PADRC'!M1)-'DRC-BDRC'!M2</f>
-        <v>185363.6363636367</v>
-      </c>
-      <c r="N2" s="6">
+        <v>126363.6363636367</v>
+      </c>
+      <c r="N2" s="4">
         <f>TREND('Data and Calculations'!$A$3:$B$3,'Data and Calculations'!$A$2:$B$2,'DRC-PADRC'!N1)-'DRC-BDRC'!N2</f>
-        <v>198000</v>
-      </c>
-      <c r="O2" s="6">
+        <v>139000</v>
+      </c>
+      <c r="O2" s="4">
         <f>TREND('Data and Calculations'!$A$3:$B$3,'Data and Calculations'!$A$2:$B$2,'DRC-PADRC'!O1)-'DRC-BDRC'!O2</f>
-        <v>210636.3636363633</v>
-      </c>
-      <c r="P2" s="6">
+        <v>151636.3636363633</v>
+      </c>
+      <c r="P2" s="4">
         <f>TREND('Data and Calculations'!$A$3:$B$3,'Data and Calculations'!$A$2:$B$2,'DRC-PADRC'!P1)-'DRC-BDRC'!P2</f>
-        <v>223272.72727273032</v>
-      </c>
-      <c r="Q2" s="6">
+        <v>164272.72727273032</v>
+      </c>
+      <c r="Q2" s="4">
         <f>TREND('Data and Calculations'!$A$3:$B$3,'Data and Calculations'!$A$2:$B$2,'DRC-PADRC'!Q1)-'DRC-BDRC'!Q2</f>
-        <v>235909.09090909362</v>
-      </c>
-      <c r="R2" s="6">
+        <v>176909.09090909362</v>
+      </c>
+      <c r="R2" s="4">
         <f>TREND('Data and Calculations'!$A$3:$B$3,'Data and Calculations'!$A$2:$B$2,'DRC-PADRC'!R1)-'DRC-BDRC'!R2</f>
-        <v>248545.45454545692</v>
-      </c>
-      <c r="S2" s="6">
+        <v>189545.45454545692</v>
+      </c>
+      <c r="S2" s="4">
         <f>TREND('Data and Calculations'!$A$3:$B$3,'Data and Calculations'!$A$2:$B$2,'DRC-PADRC'!S1)-'DRC-BDRC'!S2</f>
-        <v>261181.81818182021</v>
-      </c>
-      <c r="T2" s="6">
+        <v>202181.81818182021</v>
+      </c>
+      <c r="T2" s="4">
         <f>TREND('Data and Calculations'!$A$3:$B$3,'Data and Calculations'!$A$2:$B$2,'DRC-PADRC'!T1)-'DRC-BDRC'!T2</f>
-        <v>273818.18181818351</v>
-      </c>
-      <c r="U2" s="6">
+        <v>214818.18181818351</v>
+      </c>
+      <c r="U2" s="4">
         <f>TREND('Data and Calculations'!$A$3:$B$3,'Data and Calculations'!$A$2:$B$2,'DRC-PADRC'!U1)-'DRC-BDRC'!U2</f>
-        <v>286454.54545454681</v>
-      </c>
-      <c r="V2" s="6">
+        <v>227454.54545454681</v>
+      </c>
+      <c r="V2" s="4">
         <f>TREND('Data and Calculations'!$A$3:$B$3,'Data and Calculations'!$A$2:$B$2,'DRC-PADRC'!V1)-'DRC-BDRC'!V2</f>
-        <v>299090.90909091011</v>
-      </c>
-      <c r="W2" s="6">
+        <v>240090.90909091011</v>
+      </c>
+      <c r="W2" s="4">
         <f>TREND('Data and Calculations'!$A$3:$B$3,'Data and Calculations'!$A$2:$B$2,'DRC-PADRC'!W1)-'DRC-BDRC'!W2</f>
-        <v>311727.2727272734</v>
-      </c>
-      <c r="X2" s="6">
+        <v>252727.2727272734</v>
+      </c>
+      <c r="X2" s="4">
         <f>TREND('Data and Calculations'!$A$3:$B$3,'Data and Calculations'!$A$2:$B$2,'DRC-PADRC'!X1)-'DRC-BDRC'!X2</f>
-        <v>324363.6363636367</v>
-      </c>
-      <c r="Y2" s="6">
+        <v>265363.6363636367</v>
+      </c>
+      <c r="Y2" s="4">
         <f>TREND('Data and Calculations'!$A$3:$B$3,'Data and Calculations'!$A$2:$B$2,'DRC-PADRC'!Y1)-'DRC-BDRC'!Y2</f>
-        <v>337000</v>
-      </c>
-      <c r="Z2" s="6">
+        <v>278000</v>
+      </c>
+      <c r="Z2" s="4">
         <f>TREND('Data and Calculations'!$A$3:$B$3,'Data and Calculations'!$A$2:$B$2,'DRC-PADRC'!Z1)-'DRC-BDRC'!Z2</f>
-        <v>349636.3636363633</v>
-      </c>
-      <c r="AA2" s="6">
+        <v>290636.3636363633</v>
+      </c>
+      <c r="AA2" s="4">
         <f>TREND('Data and Calculations'!$A$3:$B$3,'Data and Calculations'!$A$2:$B$2,'DRC-PADRC'!AA1)-'DRC-BDRC'!AA2</f>
-        <v>362272.72727273032</v>
-      </c>
-      <c r="AB2" s="6">
+        <v>303272.72727273032</v>
+      </c>
+      <c r="AB2" s="4">
         <f>TREND('Data and Calculations'!$A$3:$B$3,'Data and Calculations'!$A$2:$B$2,'DRC-PADRC'!AB1)-'DRC-BDRC'!AB2</f>
-        <v>374909.09090909362</v>
-      </c>
-      <c r="AC2" s="6">
+        <v>315909.09090909362</v>
+      </c>
+      <c r="AC2" s="4">
         <f>TREND('Data and Calculations'!$A$3:$B$3,'Data and Calculations'!$A$2:$B$2,'DRC-PADRC'!AC1)-'DRC-BDRC'!AC2</f>
-        <v>387545.45454545692</v>
-      </c>
-      <c r="AD2" s="6">
+        <v>328545.45454545692</v>
+      </c>
+      <c r="AD2" s="4">
         <f>TREND('Data and Calculations'!$A$3:$B$3,'Data and Calculations'!$A$2:$B$2,'DRC-PADRC'!AD1)-'DRC-BDRC'!AD2</f>
-        <v>400181.81818182021</v>
-      </c>
-      <c r="AE2" s="6">
+        <v>341181.81818182021</v>
+      </c>
+      <c r="AE2" s="4">
         <f>TREND('Data and Calculations'!$A$3:$B$3,'Data and Calculations'!$A$2:$B$2,'DRC-PADRC'!AE1)-'DRC-BDRC'!AE2</f>
-        <v>412818.18181818351</v>
-      </c>
-      <c r="AF2" s="6">
+        <v>353818.18181818351</v>
+      </c>
+      <c r="AF2" s="4">
         <f>TREND('Data and Calculations'!$A$3:$B$3,'Data and Calculations'!$A$2:$B$2,'DRC-PADRC'!AF1)-'DRC-BDRC'!AF2</f>
-        <v>425454.54545454681</v>
-      </c>
-      <c r="AG2" s="6">
+        <v>366454.54545454681</v>
+      </c>
+      <c r="AG2" s="4">
         <f>TREND('Data and Calculations'!$A$3:$B$3,'Data and Calculations'!$A$2:$B$2,'DRC-PADRC'!AG1)-'DRC-BDRC'!AG2</f>
-        <v>438090.90909091011</v>
-      </c>
-      <c r="AH2" s="6">
+        <v>379090.90909091011</v>
+      </c>
+      <c r="AH2" s="4">
         <f>TREND('Data and Calculations'!$A$3:$B$3,'Data and Calculations'!$A$2:$B$2,'DRC-PADRC'!AH1)-'DRC-BDRC'!AH2</f>
-        <v>450727.2727272734</v>
+        <v>391727.2727272734</v>
       </c>
     </row>
   </sheetData>
@@ -1304,53 +1300,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="9" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="4">
         <f>'Data and Calculations'!A17</f>
         <v>96</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="6"/>
-      <c r="W2" s="6"/>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="6"/>
-      <c r="Z2" s="6"/>
-      <c r="AA2" s="6"/>
-      <c r="AB2" s="6"/>
-      <c r="AC2" s="6"/>
-      <c r="AD2" s="6"/>
-      <c r="AE2" s="6"/>
-      <c r="AF2" s="6"/>
-      <c r="AG2" s="6"/>
-      <c r="AH2" s="6"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="4"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="4"/>
+      <c r="AA2" s="4"/>
+      <c r="AB2" s="4"/>
+      <c r="AC2" s="4"/>
+      <c r="AD2" s="4"/>
+      <c r="AE2" s="4"/>
+      <c r="AF2" s="4"/>
+      <c r="AG2" s="4"/>
+      <c r="AH2" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1374,53 +1370,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="9" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="4">
         <f>'Data and Calculations'!A20</f>
         <v>4</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="6"/>
-      <c r="W2" s="6"/>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="6"/>
-      <c r="Z2" s="6"/>
-      <c r="AA2" s="6"/>
-      <c r="AB2" s="6"/>
-      <c r="AC2" s="6"/>
-      <c r="AD2" s="6"/>
-      <c r="AE2" s="6"/>
-      <c r="AF2" s="6"/>
-      <c r="AG2" s="6"/>
-      <c r="AH2" s="6"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="4"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="4"/>
+      <c r="AA2" s="4"/>
+      <c r="AB2" s="4"/>
+      <c r="AC2" s="4"/>
+      <c r="AD2" s="4"/>
+      <c r="AE2" s="4"/>
+      <c r="AF2" s="4"/>
+      <c r="AG2" s="4"/>
+      <c r="AH2" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Remove all unused electricity sector variables and policies
</commit_message>
<xml_diff>
--- a/InputData/elec/DRC/Demand Response Capacity.xlsx
+++ b/InputData/elec/DRC/Demand Response Capacity.xlsx
@@ -1,24 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\DRC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\DRC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E14643-8DF8-47DF-923D-41404FE63C2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845A6FAA-504D-4C75-BC8B-E953DE6936DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="26940" windowHeight="20235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Data and Calculations" sheetId="4" r:id="rId2"/>
     <sheet name="DRC-BDRC" sheetId="5" r:id="rId3"/>
     <sheet name="DRC-PADRC" sheetId="2" r:id="rId4"/>
-    <sheet name="DRC-HoDRAUMCUpY" sheetId="6" r:id="rId5"/>
-    <sheet name="DRC-ADRHpDRE" sheetId="7" r:id="rId6"/>
+    <sheet name="DRC-ADRHpDRE" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>Year</t>
   </si>
@@ -124,12 +123,6 @@
   </si>
   <si>
     <t>Hours of DR per Event</t>
-  </si>
-  <si>
-    <t>DR Hours per Year</t>
-  </si>
-  <si>
-    <t>Hours per Year</t>
   </si>
   <si>
     <t>DRC Average DR Hours per DR Event</t>
@@ -560,12 +553,12 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -653,17 +646,17 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -714,14 +707,14 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1285,7 +1278,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1FC88BD-436A-47FC-A8D1-F56A62CE3FDC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDBC3D16-B83D-4A6D-B504-E642B89301D6}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -1304,16 +1297,16 @@
         <v>15</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B2" s="4">
-        <f>'Data and Calculations'!A17</f>
-        <v>96</v>
+        <f>'Data and Calculations'!A20</f>
+        <v>4</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -1352,74 +1345,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDBC3D16-B83D-4A6D-B504-E642B89301D6}">
-  <sheetPr>
-    <tabColor theme="3"/>
-  </sheetPr>
-  <dimension ref="A1:AH2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="33.140625" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="4">
-        <f>'Data and Calculations'!A20</f>
-        <v>4</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
-      <c r="Y2" s="4"/>
-      <c r="Z2" s="4"/>
-      <c r="AA2" s="4"/>
-      <c r="AB2" s="4"/>
-      <c r="AC2" s="4"/>
-      <c r="AD2" s="4"/>
-      <c r="AE2" s="4"/>
-      <c r="AF2" s="4"/>
-      <c r="AG2" s="4"/>
-      <c r="AH2" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
CL, DRC, AVL: add 'ROUND' function to make sure output values are in integers
</commit_message>
<xml_diff>
--- a/InputData/elec/DRC/Demand Response Capacity.xlsx
+++ b/InputData/elec/DRC/Demand Response Capacity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\DRC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olivia Ashmoore\Documents\EPS_Models by Region\United States\us-eps\InputData\elec\DRC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845A6FAA-504D-4C75-BC8B-E953DE6936DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{726D1944-1CAD-447D-897B-E50B30316ACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -534,34 +534,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="2" max="2" width="107.28515625" customWidth="1"/>
+    <col min="2" max="2" width="107.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A3" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -569,92 +569,92 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.75">
       <c r="B7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.75">
       <c r="B8" s="2">
         <v>2019</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.75">
       <c r="B9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.75">
       <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.75">
       <c r="B11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.75">
       <c r="B13" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.75">
       <c r="B14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.75">
       <c r="B15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.75">
       <c r="B16" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.75">
       <c r="B17" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.75">
       <c r="B18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A20" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A21" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A22" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A25" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A26" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -677,19 +677,19 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A1" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A2">
         <v>2019</v>
       </c>
@@ -697,7 +697,7 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A3">
         <v>59000</v>
       </c>
@@ -705,44 +705,44 @@
         <v>198000</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A9" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A16" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A17">
         <v>96</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A19" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A20">
         <v>4</v>
       </c>
@@ -764,12 +764,12 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -873,7 +873,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.75">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1026,12 +1026,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1135,7 +1135,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:34" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -1284,15 +1284,17 @@
   </sheetPr>
   <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="33.140625" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="33.1328125" customWidth="1"/>
+    <col min="2" max="2" width="17.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.75">
       <c r="A1" s="8" t="s">
         <v>15</v>
       </c>
@@ -1300,12 +1302,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="4">
-        <f>'Data and Calculations'!A20</f>
+        <f>ROUND('Data and Calculations'!A20,0)</f>
         <v>4</v>
       </c>
       <c r="C2" s="4"/>

</xml_diff>